<commit_message>
success get locale without interceptor
</commit_message>
<xml_diff>
--- a/document/基本設計書.xlsx
+++ b/document/基本設計書.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\azusato\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D438372C-0692-47BF-89C3-7938D82C719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234FA171-29AE-4305-93D0-AA0B217D2961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="構成図" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1"/>
@@ -505,6 +505,49 @@
     <rPh sb="41" eb="43">
       <t>タイオウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>celebration</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>member</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>言語</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンゴ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>interceptor =&gt; posthandle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ja</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ko</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -799,13 +842,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>228601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -867,13 +910,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -927,13 +970,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -993,13 +1036,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>485776</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1059,13 +1102,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1135,13 +1178,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>657151</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>209499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1179,13 +1222,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>92916</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>190364</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1223,13 +1266,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1283,13 +1326,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1359,13 +1402,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>38101</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>54816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1403,13 +1446,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1471,14 +1514,14 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1493,8 +1536,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12363451" y="1323976"/>
-          <a:ext cx="3867150" cy="2124074"/>
+          <a:off x="12363451" y="1800226"/>
+          <a:ext cx="3867150" cy="1714499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1539,13 +1582,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>190443</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>190452</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1589,7 +1632,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1729,13 +1772,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1801,7 +1844,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1895,13 +1938,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>323801</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>199970</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2041,7 +2084,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>128563</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2094,13 +2137,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>28523</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>190455</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2138,13 +2181,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2194,13 +2237,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2274,13 +2317,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>600027</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>161883</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2318,13 +2361,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>409551</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>161883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>176213</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2377,13 +2420,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2472,13 +2515,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>486716</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>142781</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2522,7 +2565,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>567208</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2655,13 +2698,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>266701</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>131325</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>85654</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2699,13 +2742,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>471487</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2758,13 +2801,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>133349</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2892,6 +2935,132 @@
             <a:t>詳細説明は「言語」シートで</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD01170-89FC-46D2-ADCA-4A3C3981DE94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="657225" y="3819525"/>
+          <a:ext cx="6143625" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ページネーム</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rectangle 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C45FF91-6D4F-4C62-89BC-11EC1D42F11D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12372975" y="3524250"/>
+          <a:ext cx="3876675" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ページネーム</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5172,7 +5341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -5274,10 +5443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE11843-A251-4FD0-A93F-C7D2793D5A11}">
-  <dimension ref="B3:V5"/>
+  <dimension ref="B3:V12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5308,11 +5477,69 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
+      <c r="M5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" t="s">
+        <v>64</v>
+      </c>
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="M6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="S5" t="s">
+      <c r="N7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S7" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="N8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="M9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="N10" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="N11" t="s">
+        <v>67</v>
+      </c>
+      <c r="O11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="N12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>